<commit_message>
Thông tin sp 2
</commit_message>
<xml_diff>
--- a/1412570/hinhtuixach/thông tin hình ảnh.xlsx
+++ b/1412570/hinhtuixach/thông tin hình ảnh.xlsx
@@ -18,15 +18,97 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Tên sản phẩm</t>
+  </si>
+  <si>
+    <t>Loại sản phẩm</t>
+  </si>
+  <si>
+    <t>Giá</t>
+  </si>
+  <si>
+    <t>Nhà sản suất/thương hiệu</t>
+  </si>
+  <si>
+    <t>Mô tả chi tiết</t>
+  </si>
+  <si>
+    <t>Túi nhũ kim tuyến siêu sang - T478</t>
+  </si>
+  <si>
+    <t>Nguồn</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-nhu-kim-tuyen-sieu-sang-t478-i167057096-s182856632.html?spm=a2o4n.pdp.recommendation_2.2.7f0783d9H2vUvN&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=61b6562c-2de0-4f52-9c12-c4f82f011106__167057096__14248__1</t>
+  </si>
+  <si>
+    <t>Túi xách nữ/túi đeo chéo/túi đeo vai nữ</t>
+  </si>
+  <si>
+    <t>160k</t>
+  </si>
+  <si>
+    <t>OEM</t>
+  </si>
+  <si>
+    <t>Thông tin sản phẩm:
+Chất liệu: da
+ Kích thước: 20 x 5x 7cm
+Style: Korea
+Công dụng: Đi chơi, đi làm
+Túi nhũ kim tuyến siêu sang - T478 mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng. Chúng có sự đa dạng từ kiểu cách tới màu sắc, size…tùy theo nhu cầu của mình mà các nàng lựa chọn một sản phẩm thích hợp.</t>
+  </si>
+  <si>
+    <t>Đặc tính sản phẩm</t>
+  </si>
+  <si>
+    <t>SKU OE680FAAAOCCPGVNAMZ-51184554
+Địa điểm ứng dụng Phù hợp cho mọi dịp
+Dòng sản phẩmTÚI ĐEO CHÉO NỮ
+Chất liệu vải Da PU
+Xu Hướng Nữ Thường ngày,Công sở,Thời trang dạo phố,Tiệc
+Chất liệu PU
+Loại bảo hành No Warranty
+Material DaDạng 
+Túi Túi đeo vai</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +131,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +423,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.625" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="6" width="83.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
thông tin sp 3
</commit_message>
<xml_diff>
--- a/1412570/hinhtuixach/thông tin hình ảnh.xlsx
+++ b/1412570/hinhtuixach/thông tin hình ảnh.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -48,39 +48,92 @@
     <t>Túi xách nữ/túi đeo chéo/túi đeo vai nữ</t>
   </si>
   <si>
-    <t>160k</t>
-  </si>
-  <si>
     <t>OEM</t>
+  </si>
+  <si>
+    <t>Đặc tính sản phẩm</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-happy-day-tre-trung-t438-i167534394-s183358223.html?spm=a2o4n.pdp.recommendation_1.1.77de35c6OnWOoC&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=4d40f851-6071-4394-8435-c7e728a3c06d__167534394__14248__1</t>
+  </si>
+  <si>
+    <t>Túi Happy Day trẻ trung - T438</t>
   </si>
   <si>
     <t>Thông tin sản phẩm:
 Chất liệu: da
  Kích thước: 20 x 5x 7cm
+Màu sắc: Bạc, Xanh, Đen
 Style: Korea
 Công dụng: Đi chơi, đi làm
 Túi nhũ kim tuyến siêu sang - T478 mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng. Chúng có sự đa dạng từ kiểu cách tới màu sắc, size…tùy theo nhu cầu của mình mà các nàng lựa chọn một sản phẩm thích hợp.</t>
   </si>
   <si>
-    <t>Đặc tính sản phẩm</t>
-  </si>
-  <si>
-    <t>SKU OE680FAAAOCCPGVNAMZ-51184554
-Địa điểm ứng dụng Phù hợp cho mọi dịp
-Dòng sản phẩmTÚI ĐEO CHÉO NỮ
-Chất liệu vải Da PU
-Xu Hướng Nữ Thường ngày,Công sở,Thời trang dạo phố,Tiệc
-Chất liệu PU
-Loại bảo hành No Warranty
-Material DaDạng 
-Túi Túi đeo vai</t>
+    <t>Thông tin sản phẩm:
+Chất liệu: Da PU
+Kích thước: 24 x 17 x 8cm
+Màu sắc: Xanh, Hồng
+Style: Korea
+Công dụng: Đi chơi, đi làm
+Túi Happy Day trẻ trung - T438 Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng.</t>
+  </si>
+  <si>
+    <t>SKU: OE680FAAAOCCPGVNAMZ-51184554
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Xu Hướng Nữ: Thường ngày,Công sở,Thời trang dạo phố,Tiệc
+Chất liệu: PU
+Loại bảo hành: No Warranty
+Material: Da
+Dạng túi: Túi đeo vai</t>
+  </si>
+  <si>
+    <t>SKU: OE680FAAAOLI4LVNAMZ-51618966
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Xu Hướng Nữ: Thường ngày,Công sở,Thời trang dạo phố
+Chất liệu: PU
+Loại bảo hành: No Warranty
+Material: Da
+Dạng túi: Túi đeo vai</t>
+  </si>
+  <si>
+    <t>Túi hình quyển sách độc đáo - T275</t>
+  </si>
+  <si>
+    <t>Thông tin sản phẩm:
+Chất liệu: Da PU
+Màu sắc : trắng, đen
+Kích thước: 18 x 14 x 7 cm
+Style: Korea
+Công dụng: Đi chơi, đi làm
+Trong thế giới thời trang của phái đẹp, chiếc túi luôn chiếm một vị trí quan trọng. Từ những cô nàng bình thường nhất cho tới những ngôi sao hàng đầu, tất cả đều chia sẻ một tình yêu vĩ đại với những chiếc túi
+Chiếc túi xách hợp dáng người, hợp màu sắc làm tăng vẻ đẹp của trang phục bạn mặc và khẳng định ấn tượng của bạn trong mắt người đối diện. Tuy nhiên, không phải ai cũng biết chọn một chiếc túi xách thực sự phù hợp với phom cơ thể của mình.
+Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng. Chúng có sự đa dạng từ kiểu cách tới màu sắc, size…tùy theo nhu cầu của mình mà các nàng lựa chọn một sản phẩm thích hợp. 
+Và nếu bạn cũng đang đi tìm một chiếc túi có thể thể hiện được cá tính của bản thân một cách rõ nét nhất và đang... lạc lối, thì hãy cùng khám phá và cảm nhận những nét đẹp và quyến rũ</t>
+  </si>
+  <si>
+    <t>SKU: 203055335_VNAMZ-253334510
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-hinh-quyen-sach-doc-dao-t275-i203055335-s253334510.html?spm=a2o4n.pdp.recommendation_1.1.33c23b234BtxMR&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=c74abe59-3cc9-49b8-ad9d-c8bb9533d769__203055335__14248__1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +163,29 @@
       <family val="2"/>
       <charset val="163"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF212121"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,11 +193,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -141,6 +222,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -423,64 +517,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.625" customWidth="1"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="6" width="83.75" customWidth="1"/>
+    <col min="2" max="2" width="24.625" customWidth="1"/>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="83.75" customWidth="1"/>
+    <col min="7" max="7" width="57.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>160000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <v>180000</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="256.5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>100000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="128.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update đủ 10 hình
</commit_message>
<xml_diff>
--- a/1412570/hinhtuixach/thông tin hình ảnh.xlsx
+++ b/1412570/hinhtuixach/thông tin hình ảnh.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -128,12 +128,182 @@
   <si>
     <t>https://www.lazada.vn/products/tui-hinh-quyen-sach-doc-dao-t275-i203055335-s253334510.html?spm=a2o4n.pdp.recommendation_1.1.33c23b234BtxMR&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=c74abe59-3cc9-49b8-ad9d-c8bb9533d769__203055335__14248__1</t>
   </si>
+  <si>
+    <t>Túi bling bling viền ngọc trai tua rua - T201</t>
+  </si>
+  <si>
+    <t>Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng. Chúng có sự đa dạng từ kiểu cách tới màu sắc, size…tùy theo nhu cầu của mình mà các nàng lựa chọn một sản phẩm thích hợp.
+Và nếu bạn cũng đang đi tìm một chiếc túi có thể thể hiện được cá tính của bản thân một cách rõ nét nhất và đang... lạc lối, thì hãy cùng khám phá và cảm nhận những nét đẹp và quyến rũ của
+Túi bling bling viền ngọc trai tua rua - T201
+Thông tin sản phẩm:
+Chất liệu: da PU
+Màu sắc : Đen, hồng, vàng
+Kích thước: 19 x 15 x 8cm
+Style: Korea
+Công dụng: Đi chơi, đi làm</t>
+  </si>
+  <si>
+    <t>SKU: 202050857_VNAMZ-252273393
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-bling-bling-vien-ngoc-trai-tua-rua-t201-i202050857-s252273393.html?spm=a2o4n.pdp.recommendation_1.1.192531889jFGMQ&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=c832a463-d6c9-4ac0-a4b8-2e0404c1cd08__202050857__14248__1</t>
+  </si>
+  <si>
+    <t>Túi lấp lánh bling bling tua rua - T253</t>
+  </si>
+  <si>
+    <t>SKU: 203031004_VNAMZ-253311108
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-lap-lanh-bling-bling-tua-rua-t253-i203031004-s253311108.html?spm=a2o4n.pdp.recommendation_1.1.71d44e2bYIFQje&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=1bb9a985-3f03-4a21-ad1d-a5ea3a575599__203031004__14251__1</t>
+  </si>
+  <si>
+    <t>Túi da xước siêu xinh - T499</t>
+  </si>
+  <si>
+    <t>Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng. Chúng có sự đa dạng từ kiểu cách tới màu sắc, size…tùy theo nhu cầu của mình mà các nàng lựa chọn một sản phẩm thích hợp. 
+Và nếu bạn cũng đang đi tìm một chiếc túi có thể thể hiện được cá tính của bản thân một cách rõ nét nhất và đang... lạc lối, thì hãy cùng khám phá và cảm nhận những nét đẹp và quyến rũ của 
+Túi lấp lánh bling bling tua rua
+Thông tin sản phẩm:
+Chất liệu: da PU
+Màu sắc : Đen, hồng
+Kích thước: 19 x 15 x 8cm
+Style: Korea
+Công dụng: Đi chơi, đi làm</t>
+  </si>
+  <si>
+    <t>Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng
+Thông tin sản phẩm:
+Chất liệu: da PU
+Màu sắc : Đen, hồng
+Kích thước: 19 x 15 x 8cm
+Style: Korea
+Công dụng: Đi chơi, đi làm</t>
+  </si>
+  <si>
+    <t>SKU: OE680FAAANTMRWVNAMZ-50280698
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-da-xuoc-sieu-xinh-t499-i165785973-s181521196.html?spm=a2o4n.pdp.recommendation_1.2.79dd15e5u9T1pS&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=5c658563-9c2b-4509-879b-1c66dd0b9002__165785973__14248__1</t>
+  </si>
+  <si>
+    <t>Túi mini da siêu chất - T552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng. Chúng có sự đa dạng từ kiểu cách tới màu sắc, size…tùy theo nhu cầu của mình mà các nàng lựa chọn một sản phẩm thích hợp.
+Và nếu bạn cũng đang đi tìm một chiếc túi có thể thể hiện được cá tính của bản thân một cách rõ nét nhất và đang... lạc lối, thì hãy cùng khám phá và cảm nhận những nét đẹp và quyến rũ của
+Túi mini da lì siêu chất - T552
+Thông tin sản phẩm:
+Chất liệu: da PU
+Màu sắc : Đen, đỏ, xám, rêu
+Kích thước: 21 x 15 x 8cm
+Style: Korea
+</t>
+  </si>
+  <si>
+    <t>SKU: 203171059_VNAMZ-253514773
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-mini-da-sieu-chat-t552-i203171059-s253514773.html?spm=a2o4n.pdp.recommendation_1.1.7aee2cd8fnvOHA&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=b7360f9a-cc7a-461d-854c-01b0178a1b6a__203171059__14248__1</t>
+  </si>
+  <si>
+    <t>Túi mini bag - T555</t>
+  </si>
+  <si>
+    <t>Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng. Chúng có sự đa dạng từ kiểu cách tới màu sắc, size…tùy theo nhu cầu của mình mà các nàng lựa chọn một sản phẩm thích hợp.
+Và nếu bạn cũng đang đi tìm một chiếc túi có thể thể hiện được cá tính của bản thân một cách rõ nét nhất và đang... lạc lối, thì hãy cùng khám phá và cảm nhận những nét đẹp và quyến rũ của
+Túi mini bag - T555
+Thông tin sản phẩm:
+Chất liệu: Da lộn pha da
+Màu sắc : Đen, nâu
+Kích thước: 19.5 x 14 x 6cm
+Style: Korea
+Công dụng: Đi chơi, đi làm</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-mini-bag-t555-i203800292-s254100610.html?spm=a2o4n.pdp.recommendation_1.3.205d2eadjL41To&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=c3f56c68-daa7-4bdf-8d68-3e54c2901139__203800292__14248__1</t>
+  </si>
+  <si>
+    <t>SKU: 203800292_VNAMZ-254100610
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>Túi da trẻ trung - T551</t>
+  </si>
+  <si>
+    <t>Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng
+Túi da trơn trẻ trung - T551
+Thông tin sản phẩm:
+Chất liệu: da PU
+Màu sắc : Đen, nâu
+Kích thước: 18 x 15 x 7cm
+Style: KoreaCông dụng: Đi chơi, đi làm</t>
+  </si>
+  <si>
+    <t>SKU: OE680FAAANTB38VNAMZ-50264229
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-da-tre-trung-t551-i165779212-s181498390.html?spm=a2o4n.pdp.recommendation_2.3.1cc311cfYfR6X8&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=a065d271-0847-42bf-acb2-13869deef992__165779212__14248__1</t>
+  </si>
+  <si>
+    <t>Túi tua rua trẻ trung - T472</t>
+  </si>
+  <si>
+    <t>Túi tua rua trẻ trung - T472 Mang tới cho các cô nàng sự thoải mái khi đi dạo phố hoặc hẹn hò bè bạn vì không phải cầm mang những vật dụng linh tinh, chiếc túi xách đã trở thành người bạn không thể thiếu các nàng.
+Và nếu bạn cũng đang đi tìm một chiếc túi có thể thể hiện được cá tính của bản thân một cách rõ nét nhất và đang... lạc lối, thì hãy cùng khám phá và cảm nhận những nét đẹp và quyến rũ của Túi mắc tua dua trẻ trung - T472
+Thông tin sản phẩm:
+Chất liệu: Da PU
+Màu sắc : đen, trắng
+Kích thước: 18 x 16 x 7cm
+Style: Korea
+Công dụng: Đi chơi, đi làm</t>
+  </si>
+  <si>
+    <t>SKU: OE680FAAAPC5CYVNAMZ-52901607
+Địa điểm ứng dụng: Phù hợp cho mọi dịp
+Dòng sản phẩm:TÚI ĐEO CHÉO NỮ
+Chất liệu vải: Da PU
+Chất liệu: PU
+Loại bảo hành: No Warranty</t>
+  </si>
+  <si>
+    <t>https://www.lazada.vn/products/tui-tua-rua-tre-trung-t472-i169223776-s185130870.html?spm=a2o4n.pdp.recommendation_1.3.753b68c8Bu2H9C&amp;mp=1&amp;scm=1007.16389.99110.0&amp;clickTrackInfo=f7279d02-23fb-46c1-980e-2f602cb2c806__169223776__14248__1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +340,32 @@
       <family val="2"/>
       <charset val="163"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="17"/>
+      <color rgb="FF212121"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +378,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -208,11 +414,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -235,6 +454,42 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -519,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -636,39 +891,186 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="5" customFormat="1" ht="299.25" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>149000</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="185.25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>169000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
+    <row r="7" spans="1:8" s="14" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
+      <c r="B7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="14">
+        <v>100000</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:8" s="17" customFormat="1" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
+      <c r="B8" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="17">
+        <v>100000</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+    <row r="9" spans="1:8" s="20" customFormat="1" ht="299.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="20">
         <v>8</v>
       </c>
+      <c r="B9" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="20">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:8" s="17" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
         <v>9</v>
       </c>
+      <c r="B10" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="17">
+        <v>100000</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+    <row r="11" spans="1:8" s="20" customFormat="1" ht="270.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="20">
         <v>10</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="20">
+        <v>120000</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>